<commit_message>
cambios menu dias estadia
</commit_message>
<xml_diff>
--- a/app-medicine-r/modulos/data/datos_dias_estada.xlsx
+++ b/app-medicine-r/modulos/data/datos_dias_estada.xlsx
@@ -1,37 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-mvp\modulos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-medicine-r\modulos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4D54184A-A5B3-4F0C-B2F0-9C00F852E53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FBC7C9-33F9-4055-B72C-DC28BFF80187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Hoja1!$A$1:$I$145</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Hoja1!$A$1:$I$169</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - Hoja 16_Datos completos_data (1)" description="Conexión a la consulta 'Hoja 16_Datos completos_data (1)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - Hoja 16_Datos completos_data (1)" description="Conexión a la consulta 'Hoja 16_Datos completos_data (1)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Hoja 16_Datos completos_data (1)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Hoja 16_Datos completos_data (1)]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="41">
   <si>
     <t>Especialidad</t>
   </si>
@@ -131,12 +144,36 @@
   <si>
     <t>Mes</t>
   </si>
+  <si>
+    <t>CIRUGÍA GENERAL</t>
+  </si>
+  <si>
+    <t>CIRUGÍA CARDIOVASCULAR</t>
+  </si>
+  <si>
+    <t>CIRUGÍA MÁXILOFACIAL</t>
+  </si>
+  <si>
+    <t>CIRUGÍA TÓRAX</t>
+  </si>
+  <si>
+    <t>OBSTETRICIA Y GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>RESTO ESPECIALIDADES</t>
+  </si>
+  <si>
+    <t>TODAS</t>
+  </si>
+  <si>
+    <t>año 2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +308,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,8 +508,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -568,6 +630,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -613,9 +686,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -682,7 +763,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" name="Especialidad" tableColumnId="1"/>
@@ -700,18 +781,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Hoja_16_Datos_completos_data__1" displayName="Hoja_16_Datos_completos_data__1" ref="A1:I145" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I145"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Hoja_16_Datos_completos_data__1" displayName="Hoja_16_Datos_completos_data__1" ref="A1:I169" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I169" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="1" name="Especialidad" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" uniqueName="2" name="Mes" queryTableFieldId="2" dataDxfId="0"/>
-    <tableColumn id="3" uniqueName="3" name="Dias de estada promedio " queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="Dias de estada prequirurgicos totales" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name="DÍAS DE ESTADA PREQUIRÚRGICOS 15 años y más" queryTableFieldId="5"/>
-    <tableColumn id="6" uniqueName="6" name="DÍAS DE ESTADA PREQUIRÚRGICOS Menores de 15 años" queryTableFieldId="6"/>
-    <tableColumn id="7" uniqueName="7" name="PACIENTES INTERVENIDOS 15 años y más" queryTableFieldId="7"/>
-    <tableColumn id="8" uniqueName="8" name="PACIENTES INTERVENIDOS Menores de 15 años" queryTableFieldId="8"/>
-    <tableColumn id="9" uniqueName="9" name="Pacientes intervenidos totales," queryTableFieldId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Especialidad" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Mes" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Dias de estada promedio " queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Dias de estada prequirurgicos totales" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="DÍAS DE ESTADA PREQUIRÚRGICOS 15 años y más" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="DÍAS DE ESTADA PREQUIRÚRGICOS Menores de 15 años" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="PACIENTES INTERVENIDOS 15 años y más" queryTableFieldId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="PACIENTES INTERVENIDOS Menores de 15 años" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Pacientes intervenidos totales," queryTableFieldId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1013,11 +1094,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I145"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C145"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="66" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146:B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,10 +1144,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
@@ -1093,10 +1174,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -1123,10 +1204,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
@@ -1153,10 +1234,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
@@ -1183,10 +1264,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
@@ -1213,10 +1294,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -1243,10 +1324,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1273,10 +1354,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
@@ -1303,10 +1384,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10">
@@ -1333,10 +1414,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11">
@@ -1363,10 +1444,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12">
@@ -1393,10 +1474,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13">
@@ -1423,10 +1504,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="C14">
@@ -1453,10 +1534,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15">
@@ -1483,10 +1564,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16">
@@ -1513,10 +1594,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17">
@@ -1543,10 +1624,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18">
@@ -1573,10 +1654,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19">
@@ -1603,10 +1684,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1633,10 +1714,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21">
@@ -1663,10 +1744,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
@@ -1693,10 +1774,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23">
@@ -1723,10 +1804,10 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24">
@@ -1753,10 +1834,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>20</v>
       </c>
       <c r="C25">
@@ -1783,10 +1864,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26">
@@ -1813,10 +1894,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
       <c r="C27">
@@ -1843,10 +1924,10 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28">
@@ -1873,10 +1954,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>21</v>
       </c>
       <c r="C29">
@@ -1903,10 +1984,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
       <c r="C30">
@@ -1933,10 +2014,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31">
@@ -1963,10 +2044,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>21</v>
       </c>
       <c r="C32">
@@ -1993,10 +2074,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
       <c r="C33">
@@ -2023,10 +2104,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>21</v>
       </c>
       <c r="C34">
@@ -2053,10 +2134,10 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>21</v>
       </c>
       <c r="C35">
@@ -2083,10 +2164,10 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>21</v>
       </c>
       <c r="C36">
@@ -2113,10 +2194,10 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>21</v>
       </c>
       <c r="C37">
@@ -2143,10 +2224,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>22</v>
       </c>
       <c r="C38">
@@ -2173,10 +2254,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>22</v>
       </c>
       <c r="C39">
@@ -2203,10 +2284,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>22</v>
       </c>
       <c r="C40">
@@ -2233,10 +2314,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>22</v>
       </c>
       <c r="C41">
@@ -2263,10 +2344,10 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>22</v>
       </c>
       <c r="C42">
@@ -2293,10 +2374,10 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>22</v>
       </c>
       <c r="C43">
@@ -2323,10 +2404,10 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44">
@@ -2353,10 +2434,10 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>22</v>
       </c>
       <c r="C45">
@@ -2383,10 +2464,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>22</v>
       </c>
       <c r="C46">
@@ -2413,10 +2494,10 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>22</v>
       </c>
       <c r="C47">
@@ -2443,10 +2524,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>22</v>
       </c>
       <c r="C48">
@@ -2473,10 +2554,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>22</v>
       </c>
       <c r="C49">
@@ -2503,10 +2584,10 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>23</v>
       </c>
       <c r="C50">
@@ -2533,10 +2614,10 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>23</v>
       </c>
       <c r="C51">
@@ -2563,10 +2644,10 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>23</v>
       </c>
       <c r="C52">
@@ -2593,10 +2674,10 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>23</v>
       </c>
       <c r="C53">
@@ -2623,10 +2704,10 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>23</v>
       </c>
       <c r="C54">
@@ -2653,10 +2734,10 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>23</v>
       </c>
       <c r="C55">
@@ -2683,10 +2764,10 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>23</v>
       </c>
       <c r="C56">
@@ -2713,10 +2794,10 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>23</v>
       </c>
       <c r="C57">
@@ -2743,10 +2824,10 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>23</v>
       </c>
       <c r="C58">
@@ -2773,10 +2854,10 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>23</v>
       </c>
       <c r="C59">
@@ -2803,10 +2884,10 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>23</v>
       </c>
       <c r="C60">
@@ -2833,10 +2914,10 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>23</v>
       </c>
       <c r="C61">
@@ -2863,10 +2944,10 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>24</v>
       </c>
       <c r="C62">
@@ -2893,10 +2974,10 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>24</v>
       </c>
       <c r="C63">
@@ -2923,10 +3004,10 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>10</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>24</v>
       </c>
       <c r="C64">
@@ -2953,10 +3034,10 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>24</v>
       </c>
       <c r="C65">
@@ -2983,10 +3064,10 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>24</v>
       </c>
       <c r="C66">
@@ -3013,10 +3094,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>24</v>
       </c>
       <c r="C67">
@@ -3043,10 +3124,10 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>24</v>
       </c>
       <c r="C68">
@@ -3073,10 +3154,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>15</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>24</v>
       </c>
       <c r="C69">
@@ -3103,10 +3184,10 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>24</v>
       </c>
       <c r="C70">
@@ -3133,10 +3214,10 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>24</v>
       </c>
       <c r="C71">
@@ -3163,10 +3244,10 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>24</v>
       </c>
       <c r="C72">
@@ -3193,10 +3274,10 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>24</v>
       </c>
       <c r="C73">
@@ -3223,10 +3304,10 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>25</v>
       </c>
       <c r="C74">
@@ -3253,10 +3334,10 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>25</v>
       </c>
       <c r="C75">
@@ -3283,10 +3364,10 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>10</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>25</v>
       </c>
       <c r="C76">
@@ -3313,10 +3394,10 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>11</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>25</v>
       </c>
       <c r="C77">
@@ -3343,10 +3424,10 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>12</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>25</v>
       </c>
       <c r="C78">
@@ -3373,10 +3454,10 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>25</v>
       </c>
       <c r="C79">
@@ -3403,10 +3484,10 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>25</v>
       </c>
       <c r="C80">
@@ -3433,10 +3514,10 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>25</v>
       </c>
       <c r="C81">
@@ -3463,10 +3544,10 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>25</v>
       </c>
       <c r="C82">
@@ -3493,10 +3574,10 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>17</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>25</v>
       </c>
       <c r="C83">
@@ -3523,10 +3604,10 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>18</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>25</v>
       </c>
       <c r="C84">
@@ -3553,10 +3634,10 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>19</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>25</v>
       </c>
       <c r="C85">
@@ -3583,10 +3664,10 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>26</v>
       </c>
       <c r="C86">
@@ -3613,10 +3694,10 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>26</v>
       </c>
       <c r="C87">
@@ -3643,10 +3724,10 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>10</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>26</v>
       </c>
       <c r="C88">
@@ -3673,10 +3754,10 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>11</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>26</v>
       </c>
       <c r="C89">
@@ -3703,10 +3784,10 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>12</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>26</v>
       </c>
       <c r="C90">
@@ -3733,10 +3814,10 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>13</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>26</v>
       </c>
       <c r="C91">
@@ -3763,10 +3844,10 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>14</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>26</v>
       </c>
       <c r="C92">
@@ -3793,10 +3874,10 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>15</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>26</v>
       </c>
       <c r="C93">
@@ -3823,10 +3904,10 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>16</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>26</v>
       </c>
       <c r="C94">
@@ -3853,10 +3934,10 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>17</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>26</v>
       </c>
       <c r="C95">
@@ -3883,10 +3964,10 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>18</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>26</v>
       </c>
       <c r="C96">
@@ -3913,10 +3994,10 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>19</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>26</v>
       </c>
       <c r="C97">
@@ -3943,10 +4024,10 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>27</v>
       </c>
       <c r="C98">
@@ -3973,10 +4054,10 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>27</v>
       </c>
       <c r="C99">
@@ -4003,10 +4084,10 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>10</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>27</v>
       </c>
       <c r="C100">
@@ -4033,10 +4114,10 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>11</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>27</v>
       </c>
       <c r="C101">
@@ -4063,10 +4144,10 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>27</v>
       </c>
       <c r="C102">
@@ -4093,10 +4174,10 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>13</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>27</v>
       </c>
       <c r="C103">
@@ -4123,10 +4204,10 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>14</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>27</v>
       </c>
       <c r="C104">
@@ -4153,10 +4234,10 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>15</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>27</v>
       </c>
       <c r="C105">
@@ -4183,10 +4264,10 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>16</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>27</v>
       </c>
       <c r="C106">
@@ -4213,10 +4294,10 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>17</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>27</v>
       </c>
       <c r="C107">
@@ -4243,10 +4324,10 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>18</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>27</v>
       </c>
       <c r="C108">
@@ -4273,10 +4354,10 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>19</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>27</v>
       </c>
       <c r="C109">
@@ -4303,10 +4384,10 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>7</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>28</v>
       </c>
       <c r="C110">
@@ -4333,10 +4414,10 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>9</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>28</v>
       </c>
       <c r="C111">
@@ -4363,10 +4444,10 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>28</v>
       </c>
       <c r="C112">
@@ -4393,10 +4474,10 @@
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>11</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>28</v>
       </c>
       <c r="C113">
@@ -4423,10 +4504,10 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>12</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>28</v>
       </c>
       <c r="C114">
@@ -4453,10 +4534,10 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>13</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>28</v>
       </c>
       <c r="C115">
@@ -4483,10 +4564,10 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>14</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>28</v>
       </c>
       <c r="C116">
@@ -4513,10 +4594,10 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>15</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>28</v>
       </c>
       <c r="C117">
@@ -4543,10 +4624,10 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>16</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>28</v>
       </c>
       <c r="C118">
@@ -4573,10 +4654,10 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>17</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>28</v>
       </c>
       <c r="C119">
@@ -4603,10 +4684,10 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>18</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" t="s">
         <v>28</v>
       </c>
       <c r="C120">
@@ -4633,10 +4714,10 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>19</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>28</v>
       </c>
       <c r="C121">
@@ -4663,10 +4744,10 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>7</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" t="s">
         <v>29</v>
       </c>
       <c r="C122">
@@ -4693,10 +4774,10 @@
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>9</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" t="s">
         <v>29</v>
       </c>
       <c r="C123">
@@ -4723,10 +4804,10 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>10</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" t="s">
         <v>29</v>
       </c>
       <c r="C124">
@@ -4753,10 +4834,10 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" t="s">
         <v>29</v>
       </c>
       <c r="C125">
@@ -4783,10 +4864,10 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>12</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" t="s">
         <v>29</v>
       </c>
       <c r="C126">
@@ -4813,10 +4894,10 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>13</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" t="s">
         <v>29</v>
       </c>
       <c r="C127">
@@ -4843,10 +4924,10 @@
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>14</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" t="s">
         <v>29</v>
       </c>
       <c r="C128">
@@ -4873,10 +4954,10 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>15</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" t="s">
         <v>29</v>
       </c>
       <c r="C129">
@@ -4903,10 +4984,10 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>16</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" t="s">
         <v>29</v>
       </c>
       <c r="C130">
@@ -4933,10 +5014,10 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>17</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" t="s">
         <v>29</v>
       </c>
       <c r="C131">
@@ -4963,10 +5044,10 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>18</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" t="s">
         <v>29</v>
       </c>
       <c r="C132">
@@ -4993,10 +5074,10 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>19</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" t="s">
         <v>29</v>
       </c>
       <c r="C133">
@@ -5023,10 +5104,10 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>7</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" t="s">
         <v>30</v>
       </c>
       <c r="C134">
@@ -5053,10 +5134,10 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>9</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" t="s">
         <v>30</v>
       </c>
       <c r="C135">
@@ -5083,10 +5164,10 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>10</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" t="s">
         <v>30</v>
       </c>
       <c r="C136">
@@ -5113,10 +5194,10 @@
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+      <c r="A137" t="s">
         <v>11</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" t="s">
         <v>30</v>
       </c>
       <c r="C137">
@@ -5143,10 +5224,10 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+      <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" t="s">
         <v>30</v>
       </c>
       <c r="C138">
@@ -5173,10 +5254,10 @@
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
+      <c r="A139" t="s">
         <v>13</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" t="s">
         <v>30</v>
       </c>
       <c r="C139">
@@ -5203,10 +5284,10 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+      <c r="A140" t="s">
         <v>14</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>30</v>
       </c>
       <c r="C140">
@@ -5233,10 +5314,10 @@
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
+      <c r="A141" t="s">
         <v>15</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" t="s">
         <v>30</v>
       </c>
       <c r="C141">
@@ -5263,10 +5344,10 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>16</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" t="s">
         <v>30</v>
       </c>
       <c r="C142">
@@ -5293,10 +5374,10 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>17</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" t="s">
         <v>30</v>
       </c>
       <c r="C143">
@@ -5323,10 +5404,10 @@
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>18</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>30</v>
       </c>
       <c r="C144">
@@ -5353,10 +5434,10 @@
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>19</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" t="s">
         <v>30</v>
       </c>
       <c r="C145">
@@ -5382,7 +5463,464 @@
         <v>43</v>
       </c>
     </row>
+    <row r="146" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C146" s="2">
+        <v>2.6782160500000001</v>
+      </c>
+      <c r="D146" s="2">
+        <v>2209</v>
+      </c>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="I146" s="2">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C147" s="2">
+        <v>2.4746357200000002</v>
+      </c>
+      <c r="D147" s="2">
+        <v>884</v>
+      </c>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="I147" s="2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0.74773288000000004</v>
+      </c>
+      <c r="D148" s="2">
+        <v>162</v>
+      </c>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="I148" s="2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C149" s="2">
+        <v>4.99761905</v>
+      </c>
+      <c r="D149" s="2">
+        <v>195</v>
+      </c>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="I149" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C150" s="2">
+        <v>2.9123887399999999</v>
+      </c>
+      <c r="D150" s="2">
+        <v>2235</v>
+      </c>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="I150" s="2">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C151" s="2">
+        <v>2.61368146</v>
+      </c>
+      <c r="D151" s="2">
+        <v>213</v>
+      </c>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="I151" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" s="2">
+        <v>1.63445419</v>
+      </c>
+      <c r="D152" s="2">
+        <v>340</v>
+      </c>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="I152" s="2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" s="2">
+        <v>0.21066236999999999</v>
+      </c>
+      <c r="D153" s="2">
+        <v>107</v>
+      </c>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="I153" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C154" s="2">
+        <v>1.35525794</v>
+      </c>
+      <c r="D154" s="2">
+        <v>117</v>
+      </c>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="I154" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1.73792353</v>
+      </c>
+      <c r="D155" s="2">
+        <v>456</v>
+      </c>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="I155" s="2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" s="2">
+        <v>1.5402824100000001</v>
+      </c>
+      <c r="D156" s="2">
+        <v>736</v>
+      </c>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="I156" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C157" s="2">
+        <v>2.9285601200000002</v>
+      </c>
+      <c r="D157" s="2">
+        <v>1481</v>
+      </c>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="I157" s="2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="2">
+        <v>2.1256257600000001</v>
+      </c>
+      <c r="D158" s="2">
+        <v>584</v>
+      </c>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="I158" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C159" s="2">
+        <v>2.8895667199999999</v>
+      </c>
+      <c r="D159" s="2">
+        <v>514</v>
+      </c>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="I159" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C160" s="2">
+        <v>3.1124895600000002</v>
+      </c>
+      <c r="D160" s="2">
+        <v>651</v>
+      </c>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="I160" s="2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C161" s="2">
+        <v>1.5511565899999999</v>
+      </c>
+      <c r="D161" s="2">
+        <v>707</v>
+      </c>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="I161" s="2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C162" s="2">
+        <v>2.2869742400000002</v>
+      </c>
+      <c r="D162" s="2">
+        <v>971</v>
+      </c>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="I162" s="2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C163" s="2">
+        <v>1.75672808</v>
+      </c>
+      <c r="D163" s="2">
+        <v>760</v>
+      </c>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="I163" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C164" s="2">
+        <v>2.0569925100000002</v>
+      </c>
+      <c r="D164" s="2">
+        <v>903</v>
+      </c>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="I164" s="2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C165" s="2">
+        <v>2.0970800500000002</v>
+      </c>
+      <c r="D165" s="2">
+        <v>982</v>
+      </c>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="I165" s="2">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C166" s="2">
+        <v>2.0295235200000001</v>
+      </c>
+      <c r="D166" s="2">
+        <v>711</v>
+      </c>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="I166" s="2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C167" s="2">
+        <v>1.9672247</v>
+      </c>
+      <c r="D167" s="2">
+        <v>698</v>
+      </c>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="I167" s="2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C168" s="2">
+        <v>2.2767201799999999</v>
+      </c>
+      <c r="D168" s="2">
+        <v>899</v>
+      </c>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="I168" s="2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C169" s="2">
+        <v>1.68133255</v>
+      </c>
+      <c r="D169" s="2">
+        <v>755</v>
+      </c>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="I169" s="2">
+        <v>457</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>